<commit_message>
second commit add primary code logic
</commit_message>
<xml_diff>
--- a/表格模板.xlsx
+++ b/表格模板.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\Coding\4_PythonProject\AutoInputBom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B69451E-9E41-4D33-A76C-0E8E998CE61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76354B7-EDE6-4092-B556-8E273AB60A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,14 +31,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,6 +88,14 @@
   </si>
   <si>
     <t>ccccc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>产品编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -425,7 +425,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A2:A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -437,68 +437,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>